<commit_message>
Update Class Race Rules
</commit_message>
<xml_diff>
--- a/Sunken Temple/Ideas/Sunken Temple.xlsx
+++ b/Sunken Temple/Ideas/Sunken Temple.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="60" windowWidth="3075" windowHeight="11745" tabRatio="500"/>
+    <workbookView xWindow="-240" yWindow="0" windowWidth="25820" windowHeight="14640" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="76">
   <si>
     <t>Dwarf</t>
   </si>
@@ -166,9 +166,6 @@
   </si>
   <si>
     <t>Blood Oath Contract</t>
-  </si>
-  <si>
-    <t>.+4 Attack Power</t>
   </si>
   <si>
     <t>Volcanic Pressure</t>
@@ -528,29 +525,29 @@
     <xf numFmtId="0" fontId="3" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -945,22 +942,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C3:J46"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F36" sqref="F36"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="3" max="3" width="21.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.125" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.125" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="58.875" customWidth="1"/>
-    <col min="7" max="7" width="9.375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="14.875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="58.83203125" customWidth="1"/>
+    <col min="7" max="7" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="3:10">
       <c r="C3" s="1"/>
       <c r="D3" s="3" t="s">
         <v>6</v>
@@ -984,7 +981,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="3:10">
       <c r="C4" s="2" t="s">
         <v>13</v>
       </c>
@@ -996,19 +993,19 @@
       <c r="I4" s="8"/>
       <c r="J4" s="8"/>
     </row>
-    <row r="5" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="3:10">
       <c r="C5" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="D5" s="7"/>
-      <c r="E5" s="6"/>
+      <c r="D5" s="6"/>
+      <c r="E5" s="7"/>
       <c r="F5" s="6"/>
       <c r="G5" s="7"/>
       <c r="H5" s="7"/>
       <c r="I5" s="7"/>
-      <c r="J5" s="5"/>
-    </row>
-    <row r="6" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="J5" s="6"/>
+    </row>
+    <row r="6" spans="3:10">
       <c r="C6" s="2" t="s">
         <v>15</v>
       </c>
@@ -1020,7 +1017,7 @@
       <c r="I6" s="7"/>
       <c r="J6" s="6"/>
     </row>
-    <row r="7" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="3:10">
       <c r="C7" s="2" t="s">
         <v>1</v>
       </c>
@@ -1034,19 +1031,19 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="3:10">
       <c r="C8" s="2" t="s">
         <v>2</v>
       </c>
       <c r="D8" s="7"/>
-      <c r="E8" s="7"/>
+      <c r="E8" s="6"/>
       <c r="F8" s="5"/>
       <c r="G8" s="5"/>
       <c r="H8" s="7"/>
-      <c r="I8" s="5"/>
+      <c r="I8" s="7"/>
       <c r="J8" s="7"/>
     </row>
-    <row r="9" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="3:10">
       <c r="C9" s="2" t="s">
         <v>3</v>
       </c>
@@ -1058,19 +1055,19 @@
       <c r="I9" s="5"/>
       <c r="J9" s="7"/>
     </row>
-    <row r="10" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="3:10">
       <c r="C10" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D10" s="5"/>
+      <c r="D10" s="7"/>
       <c r="E10" s="7"/>
       <c r="F10" s="7"/>
       <c r="G10" s="5"/>
       <c r="H10" s="6"/>
-      <c r="I10" s="7"/>
+      <c r="I10" s="6"/>
       <c r="J10" s="7"/>
     </row>
-    <row r="11" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="3:10">
       <c r="C11" s="2" t="s">
         <v>5</v>
       </c>
@@ -1080,14 +1077,12 @@
       <c r="G11" s="7"/>
       <c r="H11" s="5"/>
       <c r="I11" s="6"/>
-      <c r="J11" s="5" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="12" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="J11" s="5"/>
+    </row>
+    <row r="12" spans="3:10">
       <c r="D12" s="11"/>
     </row>
-    <row r="14" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="3:10">
       <c r="C14" s="15" t="s">
         <v>36</v>
       </c>
@@ -1104,55 +1099,55 @@
         <v>27</v>
       </c>
     </row>
-    <row r="15" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C15" s="22" t="s">
+    <row r="15" spans="3:10">
+      <c r="C15" s="20" t="s">
         <v>43</v>
       </c>
-      <c r="D15" s="22" t="s">
+      <c r="D15" s="20" t="s">
         <v>0</v>
       </c>
       <c r="E15" s="13" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F15" s="10" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="G15" s="4"/>
     </row>
-    <row r="16" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C16" s="23"/>
-      <c r="D16" s="23"/>
+    <row r="16" spans="3:10">
+      <c r="C16" s="21"/>
+      <c r="D16" s="21"/>
       <c r="E16" s="3"/>
       <c r="F16" s="10"/>
       <c r="G16" s="4"/>
     </row>
-    <row r="17" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C17" s="22" t="s">
+    <row r="17" spans="3:7">
+      <c r="C17" s="20" t="s">
         <v>42</v>
       </c>
-      <c r="D17" s="22" t="s">
+      <c r="D17" s="20" t="s">
         <v>1</v>
       </c>
       <c r="E17" s="13" t="s">
+        <v>67</v>
+      </c>
+      <c r="F17" s="10" t="s">
         <v>68</v>
       </c>
-      <c r="F17" s="10" t="s">
-        <v>69</v>
-      </c>
       <c r="G17" s="4"/>
     </row>
-    <row r="18" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C18" s="23"/>
-      <c r="D18" s="23"/>
+    <row r="18" spans="3:7">
+      <c r="C18" s="21"/>
+      <c r="D18" s="21"/>
       <c r="E18" s="3"/>
       <c r="F18" s="10"/>
       <c r="G18" s="4"/>
     </row>
-    <row r="19" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C19" s="22" t="s">
+    <row r="19" spans="3:7">
+      <c r="C19" s="20" t="s">
         <v>45</v>
       </c>
-      <c r="D19" s="22" t="s">
+      <c r="D19" s="20" t="s">
         <v>15</v>
       </c>
       <c r="E19" s="13" t="s">
@@ -1163,33 +1158,33 @@
       </c>
       <c r="G19" s="4"/>
     </row>
-    <row r="20" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C20" s="27"/>
-      <c r="D20" s="27"/>
+    <row r="20" spans="3:7">
+      <c r="C20" s="22"/>
+      <c r="D20" s="22"/>
       <c r="E20" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="F20" s="10" t="s">
         <v>50</v>
       </c>
-      <c r="F20" s="10" t="s">
-        <v>51</v>
-      </c>
       <c r="G20" s="4"/>
     </row>
-    <row r="21" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="3:7">
       <c r="C21" s="16"/>
       <c r="D21" s="16"/>
       <c r="E21" s="12" t="s">
         <v>26</v>
       </c>
       <c r="F21" s="10" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="G21" s="4"/>
     </row>
-    <row r="22" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="3:7">
       <c r="C22" s="28" t="s">
         <v>35</v>
       </c>
-      <c r="D22" s="22" t="s">
+      <c r="D22" s="20" t="s">
         <v>2</v>
       </c>
       <c r="E22" s="13" t="s">
@@ -1200,18 +1195,18 @@
       </c>
       <c r="G22" s="4"/>
     </row>
-    <row r="23" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="3:7">
       <c r="C23" s="28"/>
-      <c r="D23" s="23"/>
+      <c r="D23" s="21"/>
       <c r="E23" s="3"/>
       <c r="F23" s="10"/>
       <c r="G23" s="4"/>
     </row>
-    <row r="24" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="3:7">
       <c r="C24" s="28" t="s">
         <v>47</v>
       </c>
-      <c r="D24" s="22" t="s">
+      <c r="D24" s="20" t="s">
         <v>3</v>
       </c>
       <c r="E24" s="13" t="s">
@@ -1222,18 +1217,18 @@
       </c>
       <c r="G24" s="4"/>
     </row>
-    <row r="25" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="3:7">
       <c r="C25" s="28"/>
-      <c r="D25" s="23"/>
+      <c r="D25" s="21"/>
       <c r="E25" s="3"/>
       <c r="F25" s="10"/>
       <c r="G25" s="4"/>
     </row>
-    <row r="26" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="26" spans="3:7">
       <c r="C26" s="28" t="s">
         <v>34</v>
       </c>
-      <c r="D26" s="22" t="s">
+      <c r="D26" s="20" t="s">
         <v>4</v>
       </c>
       <c r="E26" s="13" t="s">
@@ -1244,22 +1239,22 @@
       </c>
       <c r="G26" s="4"/>
     </row>
-    <row r="27" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="27" spans="3:7">
       <c r="C27" s="28"/>
-      <c r="D27" s="23"/>
+      <c r="D27" s="21"/>
       <c r="E27" s="12" t="s">
         <v>33</v>
       </c>
       <c r="F27" s="10" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="G27" s="4"/>
     </row>
-    <row r="28" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C28" s="22" t="s">
+    <row r="28" spans="3:7">
+      <c r="C28" s="20" t="s">
         <v>39</v>
       </c>
-      <c r="D28" s="22" t="s">
+      <c r="D28" s="20" t="s">
         <v>5</v>
       </c>
       <c r="E28" s="13" t="s">
@@ -1270,212 +1265,212 @@
       </c>
       <c r="G28" s="4"/>
     </row>
-    <row r="29" spans="3:7" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="C29" s="23"/>
-      <c r="D29" s="23"/>
+    <row r="29" spans="3:7" ht="47.25">
+      <c r="C29" s="21"/>
+      <c r="D29" s="21"/>
       <c r="E29" s="18" t="s">
+        <v>54</v>
+      </c>
+      <c r="F29" s="17" t="s">
         <v>55</v>
       </c>
-      <c r="F29" s="17" t="s">
-        <v>56</v>
-      </c>
       <c r="G29" s="4"/>
     </row>
-    <row r="30" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C30" s="20" t="s">
+    <row r="30" spans="3:7">
+      <c r="C30" s="23" t="s">
         <v>37</v>
       </c>
-      <c r="D30" s="20" t="s">
+      <c r="D30" s="23" t="s">
         <v>6</v>
       </c>
       <c r="E30" s="3"/>
       <c r="F30" s="10"/>
       <c r="G30" s="4"/>
     </row>
-    <row r="31" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="31" spans="3:7">
       <c r="C31" s="24"/>
       <c r="D31" s="24"/>
       <c r="E31" s="12" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F31" s="10"/>
       <c r="G31" s="4"/>
     </row>
-    <row r="32" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C32" s="21"/>
-      <c r="D32" s="21"/>
+    <row r="32" spans="3:7">
+      <c r="C32" s="25"/>
+      <c r="D32" s="25"/>
       <c r="E32" s="12" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F32" s="10"/>
       <c r="G32" s="4"/>
     </row>
-    <row r="33" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C33" s="20" t="s">
+    <row r="33" spans="3:7">
+      <c r="C33" s="23" t="s">
         <v>40</v>
       </c>
-      <c r="D33" s="20" t="s">
+      <c r="D33" s="23" t="s">
         <v>11</v>
       </c>
       <c r="E33" s="13" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F33" s="10"/>
       <c r="G33" s="4"/>
     </row>
-    <row r="34" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C34" s="21"/>
-      <c r="D34" s="21"/>
+    <row r="34" spans="3:7">
+      <c r="C34" s="25"/>
+      <c r="D34" s="25"/>
       <c r="E34" s="19" t="s">
         <v>32</v>
       </c>
       <c r="F34" s="10" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G34" s="4"/>
     </row>
-    <row r="35" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C35" s="25" t="s">
+    <row r="35" spans="3:7">
+      <c r="C35" s="26" t="s">
         <v>41</v>
       </c>
-      <c r="D35" s="20" t="s">
+      <c r="D35" s="23" t="s">
         <v>8</v>
       </c>
       <c r="E35" s="3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F35" s="10"/>
       <c r="G35" s="4"/>
     </row>
-    <row r="36" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C36" s="26"/>
-      <c r="D36" s="21"/>
+    <row r="36" spans="3:7">
+      <c r="C36" s="27"/>
+      <c r="D36" s="25"/>
       <c r="E36" s="12" t="s">
         <v>32</v>
       </c>
       <c r="F36" s="10"/>
       <c r="G36" s="4"/>
     </row>
-    <row r="37" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C37" s="20" t="s">
+    <row r="37" spans="3:7">
+      <c r="C37" s="23" t="s">
         <v>38</v>
       </c>
-      <c r="D37" s="20" t="s">
+      <c r="D37" s="23" t="s">
         <v>19</v>
       </c>
       <c r="E37" s="3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="F37" s="10"/>
       <c r="G37" s="4"/>
     </row>
-    <row r="38" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C38" s="21"/>
-      <c r="D38" s="21"/>
+    <row r="38" spans="3:7">
+      <c r="C38" s="25"/>
+      <c r="D38" s="25"/>
       <c r="E38" s="3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F38" s="10"/>
       <c r="G38" s="4"/>
     </row>
-    <row r="39" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C39" s="20" t="s">
+    <row r="39" spans="3:7">
+      <c r="C39" s="23" t="s">
         <v>46</v>
       </c>
-      <c r="D39" s="20" t="s">
+      <c r="D39" s="23" t="s">
         <v>12</v>
       </c>
       <c r="E39" s="13" t="s">
+        <v>62</v>
+      </c>
+      <c r="F39" s="10" t="s">
+        <v>64</v>
+      </c>
+      <c r="G39" s="4"/>
+    </row>
+    <row r="40" spans="3:7" ht="47.25">
+      <c r="C40" s="25"/>
+      <c r="D40" s="25"/>
+      <c r="E40" s="18" t="s">
         <v>63</v>
       </c>
-      <c r="F39" s="10" t="s">
-        <v>65</v>
-      </c>
-      <c r="G39" s="4"/>
-    </row>
-    <row r="40" spans="3:7" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="C40" s="21"/>
-      <c r="D40" s="21"/>
-      <c r="E40" s="18" t="s">
-        <v>64</v>
-      </c>
       <c r="F40" s="17" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G40" s="4"/>
     </row>
-    <row r="41" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C41" s="20" t="s">
+    <row r="41" spans="3:7">
+      <c r="C41" s="23" t="s">
         <v>48</v>
       </c>
-      <c r="D41" s="20" t="s">
+      <c r="D41" s="23" t="s">
         <v>9</v>
       </c>
       <c r="E41" s="13" t="s">
+        <v>59</v>
+      </c>
+      <c r="F41" s="10" t="s">
         <v>60</v>
       </c>
-      <c r="F41" s="10" t="s">
-        <v>61</v>
-      </c>
       <c r="G41" s="4"/>
     </row>
-    <row r="42" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="42" spans="3:7">
       <c r="C42" s="24"/>
       <c r="D42" s="24"/>
       <c r="E42" s="12" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="F42" s="10"/>
       <c r="G42" s="4"/>
     </row>
-    <row r="43" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="43" spans="3:7">
       <c r="C43" s="24"/>
       <c r="D43" s="24"/>
       <c r="E43" s="12" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F43" s="10"/>
       <c r="G43" s="4"/>
     </row>
-    <row r="44" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C44" s="21"/>
-      <c r="D44" s="21"/>
+    <row r="44" spans="3:7">
+      <c r="C44" s="25"/>
+      <c r="D44" s="25"/>
       <c r="E44" s="12" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F44" s="10"/>
       <c r="G44" s="4"/>
     </row>
-    <row r="45" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C45" s="20" t="s">
+    <row r="45" spans="3:7">
+      <c r="C45" s="23" t="s">
         <v>44</v>
       </c>
-      <c r="D45" s="20" t="s">
+      <c r="D45" s="23" t="s">
         <v>10</v>
       </c>
       <c r="E45" s="13" t="s">
         <v>25</v>
       </c>
       <c r="F45" s="10" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="G45" s="4"/>
     </row>
-    <row r="46" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C46" s="21"/>
-      <c r="D46" s="21"/>
+    <row r="46" spans="3:7">
+      <c r="C46" s="25"/>
+      <c r="D46" s="25"/>
       <c r="E46" s="3"/>
       <c r="F46" s="10"/>
       <c r="G46" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="28">
-    <mergeCell ref="D17:D18"/>
-    <mergeCell ref="C19:C20"/>
-    <mergeCell ref="C28:C29"/>
-    <mergeCell ref="C30:C32"/>
-    <mergeCell ref="C33:C34"/>
-    <mergeCell ref="D22:D23"/>
+    <mergeCell ref="C45:C46"/>
+    <mergeCell ref="D24:D25"/>
+    <mergeCell ref="D26:D27"/>
+    <mergeCell ref="D28:D29"/>
+    <mergeCell ref="D39:D40"/>
+    <mergeCell ref="D45:D46"/>
     <mergeCell ref="D15:D16"/>
     <mergeCell ref="D41:D44"/>
     <mergeCell ref="D37:D38"/>
@@ -1492,15 +1487,14 @@
     <mergeCell ref="C26:C27"/>
     <mergeCell ref="C24:C25"/>
     <mergeCell ref="C22:C23"/>
-    <mergeCell ref="C45:C46"/>
-    <mergeCell ref="D24:D25"/>
-    <mergeCell ref="D26:D27"/>
-    <mergeCell ref="D28:D29"/>
-    <mergeCell ref="D39:D40"/>
-    <mergeCell ref="D45:D46"/>
+    <mergeCell ref="D17:D18"/>
+    <mergeCell ref="C19:C20"/>
+    <mergeCell ref="C28:C29"/>
+    <mergeCell ref="C30:C32"/>
+    <mergeCell ref="C33:C34"/>
+    <mergeCell ref="D22:D23"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
Whole bunch of mostly empty race/class classes/items.
</commit_message>
<xml_diff>
--- a/Sunken Temple/Ideas/Sunken Temple.xlsx
+++ b/Sunken Temple/Ideas/Sunken Temple.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-240" yWindow="0" windowWidth="25820" windowHeight="14640" tabRatio="500"/>
+    <workbookView xWindow="-240" yWindow="60" windowWidth="25815" windowHeight="14580" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -84,18 +84,9 @@
     <t>Multiple Arms</t>
   </si>
   <si>
-    <t>.+3 to Escape</t>
-  </si>
-  <si>
-    <t>.+2 Arms</t>
-  </si>
-  <si>
     <t>Precision</t>
   </si>
   <si>
-    <t>.+2 Attack Power</t>
-  </si>
-  <si>
     <t>Strength</t>
   </si>
   <si>
@@ -174,21 +165,12 @@
     <t>Ability to make a diamond when 1 of each color gemstone is combined</t>
   </si>
   <si>
-    <t>.x2 the gemstones when receiving them from a chest</t>
-  </si>
-  <si>
     <t>Gem Finder</t>
   </si>
   <si>
-    <t>.+ 1 to Attack Power, +1 to Escape</t>
-  </si>
-  <si>
     <t>First Strike</t>
   </si>
   <si>
-    <t>Emotionless, you do not hesistate. If you are beating a monster at the beggining of a battle you can terminate it immediately. No one can interfer. Monsters can still try to run. (cannot be used to win)</t>
-  </si>
-  <si>
     <t xml:space="preserve">For a price (insert here) you can see into the future. This includes, the ability to know what type a temple guardian is and whether or not a chest is good or bad. </t>
   </si>
   <si>
@@ -201,33 +183,18 @@
     <t>Stealth</t>
   </si>
   <si>
-    <t>.+2 to Escape</t>
-  </si>
-  <si>
     <t>Master of Disguise</t>
   </si>
   <si>
-    <t>Prophetic</t>
-  </si>
-  <si>
     <t>Foresight</t>
   </si>
   <si>
     <t>Cannot be surprised. (insert here)</t>
   </si>
   <si>
-    <t>.+3 Attack Power per monster</t>
-  </si>
-  <si>
     <t>In tune with Nature</t>
   </si>
   <si>
-    <t>Agile</t>
-  </si>
-  <si>
-    <t>.+2 attack Power</t>
-  </si>
-  <si>
     <t>One-shots are worth double</t>
   </si>
   <si>
@@ -247,6 +214,39 @@
   </si>
   <si>
     <t>Growth</t>
+  </si>
+  <si>
+    <t>+3 to Escape</t>
+  </si>
+  <si>
+    <t>+2 Arms</t>
+  </si>
+  <si>
+    <t>+ 1 to Attack Power, +1 to Escape</t>
+  </si>
+  <si>
+    <t>+2 Attack Power</t>
+  </si>
+  <si>
+    <t>x2 the gemstones when receiving them from a chest</t>
+  </si>
+  <si>
+    <t>+2 attack Power</t>
+  </si>
+  <si>
+    <t>Emotionless, you do not hesistate. If you are beating a monster at the beginning of a battle you can terminate it immediately. No one can interfere. Monsters can still try to run. (cannot be used to win)</t>
+  </si>
+  <si>
+    <t>+2 to Escape</t>
+  </si>
+  <si>
+    <t>+3 Attack Power per monster</t>
+  </si>
+  <si>
+    <t>Third Eye</t>
+  </si>
+  <si>
+    <t>Agility</t>
   </si>
 </sst>
 </file>
@@ -468,7 +468,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -525,32 +525,35 @@
     <xf numFmtId="0" fontId="3" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="53">
@@ -942,22 +945,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C3:J46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+    <sheetView tabSelected="1" topLeftCell="B25" workbookViewId="0">
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="21.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="58.83203125" customWidth="1"/>
-    <col min="7" max="7" width="9.33203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.1640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="14.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.125" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="58.875" customWidth="1"/>
+    <col min="7" max="7" width="9.375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="3:10">
+    <row r="3" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C3" s="1"/>
       <c r="D3" s="3" t="s">
         <v>6</v>
@@ -981,7 +984,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="3:10">
+    <row r="4" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C4" s="2" t="s">
         <v>13</v>
       </c>
@@ -993,7 +996,7 @@
       <c r="I4" s="8"/>
       <c r="J4" s="8"/>
     </row>
-    <row r="5" spans="3:10">
+    <row r="5" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C5" s="2" t="s">
         <v>0</v>
       </c>
@@ -1005,7 +1008,7 @@
       <c r="I5" s="7"/>
       <c r="J5" s="6"/>
     </row>
-    <row r="6" spans="3:10">
+    <row r="6" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C6" s="2" t="s">
         <v>15</v>
       </c>
@@ -1017,7 +1020,7 @@
       <c r="I6" s="7"/>
       <c r="J6" s="6"/>
     </row>
-    <row r="7" spans="3:10">
+    <row r="7" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C7" s="2" t="s">
         <v>1</v>
       </c>
@@ -1031,7 +1034,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="3:10">
+    <row r="8" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C8" s="2" t="s">
         <v>2</v>
       </c>
@@ -1043,7 +1046,7 @@
       <c r="I8" s="7"/>
       <c r="J8" s="7"/>
     </row>
-    <row r="9" spans="3:10">
+    <row r="9" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C9" s="2" t="s">
         <v>3</v>
       </c>
@@ -1055,7 +1058,7 @@
       <c r="I9" s="5"/>
       <c r="J9" s="7"/>
     </row>
-    <row r="10" spans="3:10">
+    <row r="10" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C10" s="2" t="s">
         <v>4</v>
       </c>
@@ -1067,7 +1070,7 @@
       <c r="I10" s="6"/>
       <c r="J10" s="7"/>
     </row>
-    <row r="11" spans="3:10">
+    <row r="11" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C11" s="2" t="s">
         <v>5</v>
       </c>
@@ -1079,12 +1082,12 @@
       <c r="I11" s="6"/>
       <c r="J11" s="5"/>
     </row>
-    <row r="12" spans="3:10">
+    <row r="12" spans="3:10" x14ac:dyDescent="0.25">
       <c r="D12" s="11"/>
     </row>
-    <row r="14" spans="3:10">
+    <row r="14" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C14" s="15" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="D14" s="9" t="s">
         <v>18</v>
@@ -1096,381 +1099,381 @@
         <v>17</v>
       </c>
       <c r="G14" s="9" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="15" spans="3:10">
-      <c r="C15" s="20" t="s">
-        <v>43</v>
-      </c>
-      <c r="D15" s="20" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="15" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C15" s="22" t="s">
+        <v>40</v>
+      </c>
+      <c r="D15" s="22" t="s">
         <v>0</v>
       </c>
       <c r="E15" s="13" t="s">
-        <v>52</v>
-      </c>
-      <c r="F15" s="10" t="s">
-        <v>51</v>
+        <v>48</v>
+      </c>
+      <c r="F15" s="29" t="s">
+        <v>69</v>
       </c>
       <c r="G15" s="4"/>
     </row>
-    <row r="16" spans="3:10">
-      <c r="C16" s="21"/>
-      <c r="D16" s="21"/>
+    <row r="16" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C16" s="23"/>
+      <c r="D16" s="23"/>
       <c r="E16" s="3"/>
       <c r="F16" s="10"/>
       <c r="G16" s="4"/>
     </row>
-    <row r="17" spans="3:7">
-      <c r="C17" s="20" t="s">
-        <v>42</v>
-      </c>
-      <c r="D17" s="20" t="s">
+    <row r="17" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C17" s="22" t="s">
+        <v>39</v>
+      </c>
+      <c r="D17" s="22" t="s">
         <v>1</v>
       </c>
       <c r="E17" s="13" t="s">
-        <v>67</v>
-      </c>
-      <c r="F17" s="10" t="s">
-        <v>68</v>
+        <v>75</v>
+      </c>
+      <c r="F17" s="29" t="s">
+        <v>70</v>
       </c>
       <c r="G17" s="4"/>
     </row>
-    <row r="18" spans="3:7">
-      <c r="C18" s="21"/>
-      <c r="D18" s="21"/>
+    <row r="18" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C18" s="23"/>
+      <c r="D18" s="23"/>
       <c r="E18" s="3"/>
       <c r="F18" s="10"/>
       <c r="G18" s="4"/>
     </row>
-    <row r="19" spans="3:7">
-      <c r="C19" s="20" t="s">
-        <v>45</v>
-      </c>
-      <c r="D19" s="20" t="s">
+    <row r="19" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C19" s="22" t="s">
+        <v>42</v>
+      </c>
+      <c r="D19" s="22" t="s">
         <v>15</v>
       </c>
       <c r="E19" s="13" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="F19" s="10" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="G19" s="4"/>
     </row>
-    <row r="20" spans="3:7">
-      <c r="C20" s="22"/>
-      <c r="D20" s="22"/>
+    <row r="20" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C20" s="27"/>
+      <c r="D20" s="27"/>
       <c r="E20" s="12" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="F20" s="10" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="G20" s="4"/>
     </row>
-    <row r="21" spans="3:7">
+    <row r="21" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C21" s="16"/>
       <c r="D21" s="16"/>
       <c r="E21" s="12" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="F21" s="10" t="s">
-        <v>69</v>
+        <v>58</v>
       </c>
       <c r="G21" s="4"/>
     </row>
-    <row r="22" spans="3:7">
+    <row r="22" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C22" s="28" t="s">
-        <v>35</v>
-      </c>
-      <c r="D22" s="20" t="s">
+        <v>32</v>
+      </c>
+      <c r="D22" s="22" t="s">
         <v>2</v>
       </c>
       <c r="E22" s="13" t="s">
         <v>14</v>
       </c>
       <c r="F22" s="10" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="G22" s="4"/>
     </row>
-    <row r="23" spans="3:7">
+    <row r="23" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C23" s="28"/>
-      <c r="D23" s="21"/>
+      <c r="D23" s="23"/>
       <c r="E23" s="3"/>
       <c r="F23" s="10"/>
       <c r="G23" s="4"/>
     </row>
-    <row r="24" spans="3:7">
+    <row r="24" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C24" s="28" t="s">
-        <v>47</v>
-      </c>
-      <c r="D24" s="20" t="s">
+        <v>44</v>
+      </c>
+      <c r="D24" s="22" t="s">
         <v>3</v>
       </c>
       <c r="E24" s="13" t="s">
-        <v>29</v>
-      </c>
-      <c r="F24" s="10" t="s">
-        <v>21</v>
+        <v>26</v>
+      </c>
+      <c r="F24" s="29" t="s">
+        <v>65</v>
       </c>
       <c r="G24" s="4"/>
     </row>
-    <row r="25" spans="3:7">
+    <row r="25" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C25" s="28"/>
-      <c r="D25" s="21"/>
+      <c r="D25" s="23"/>
       <c r="E25" s="3"/>
       <c r="F25" s="10"/>
       <c r="G25" s="4"/>
     </row>
-    <row r="26" spans="3:7">
+    <row r="26" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C26" s="28" t="s">
-        <v>34</v>
-      </c>
-      <c r="D26" s="20" t="s">
+        <v>31</v>
+      </c>
+      <c r="D26" s="22" t="s">
         <v>4</v>
       </c>
       <c r="E26" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="F26" s="10" t="s">
-        <v>22</v>
+      <c r="F26" s="29" t="s">
+        <v>66</v>
       </c>
       <c r="G26" s="4"/>
     </row>
-    <row r="27" spans="3:7">
+    <row r="27" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C27" s="28"/>
-      <c r="D27" s="21"/>
+      <c r="D27" s="23"/>
       <c r="E27" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="F27" s="10" t="s">
-        <v>53</v>
+        <v>30</v>
+      </c>
+      <c r="F27" s="29" t="s">
+        <v>67</v>
       </c>
       <c r="G27" s="4"/>
     </row>
-    <row r="28" spans="3:7">
-      <c r="C28" s="20" t="s">
-        <v>39</v>
-      </c>
-      <c r="D28" s="20" t="s">
+    <row r="28" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C28" s="22" t="s">
+        <v>36</v>
+      </c>
+      <c r="D28" s="22" t="s">
         <v>5</v>
       </c>
       <c r="E28" s="13" t="s">
-        <v>23</v>
-      </c>
-      <c r="F28" s="10" t="s">
-        <v>24</v>
+        <v>21</v>
+      </c>
+      <c r="F28" s="29" t="s">
+        <v>68</v>
       </c>
       <c r="G28" s="4"/>
     </row>
-    <row r="29" spans="3:7" ht="47.25">
-      <c r="C29" s="21"/>
-      <c r="D29" s="21"/>
+    <row r="29" spans="3:7" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="C29" s="23"/>
+      <c r="D29" s="23"/>
       <c r="E29" s="18" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="F29" s="17" t="s">
-        <v>55</v>
+        <v>71</v>
       </c>
       <c r="G29" s="4"/>
     </row>
-    <row r="30" spans="3:7">
-      <c r="C30" s="23" t="s">
-        <v>37</v>
-      </c>
-      <c r="D30" s="23" t="s">
+    <row r="30" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C30" s="20" t="s">
+        <v>34</v>
+      </c>
+      <c r="D30" s="20" t="s">
         <v>6</v>
       </c>
       <c r="E30" s="3"/>
       <c r="F30" s="10"/>
       <c r="G30" s="4"/>
     </row>
-    <row r="31" spans="3:7">
+    <row r="31" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C31" s="24"/>
       <c r="D31" s="24"/>
       <c r="E31" s="12" t="s">
-        <v>72</v>
+        <v>61</v>
       </c>
       <c r="F31" s="10"/>
       <c r="G31" s="4"/>
     </row>
-    <row r="32" spans="3:7">
-      <c r="C32" s="25"/>
-      <c r="D32" s="25"/>
+    <row r="32" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C32" s="21"/>
+      <c r="D32" s="21"/>
       <c r="E32" s="12" t="s">
-        <v>71</v>
+        <v>60</v>
       </c>
       <c r="F32" s="10"/>
       <c r="G32" s="4"/>
     </row>
-    <row r="33" spans="3:7">
-      <c r="C33" s="23" t="s">
-        <v>40</v>
-      </c>
-      <c r="D33" s="23" t="s">
+    <row r="33" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C33" s="20" t="s">
+        <v>37</v>
+      </c>
+      <c r="D33" s="20" t="s">
         <v>11</v>
       </c>
       <c r="E33" s="13" t="s">
-        <v>73</v>
+        <v>62</v>
       </c>
       <c r="F33" s="10"/>
       <c r="G33" s="4"/>
     </row>
-    <row r="34" spans="3:7">
-      <c r="C34" s="25"/>
-      <c r="D34" s="25"/>
+    <row r="34" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C34" s="21"/>
+      <c r="D34" s="21"/>
       <c r="E34" s="19" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="F34" s="10" t="s">
-        <v>74</v>
+        <v>63</v>
       </c>
       <c r="G34" s="4"/>
     </row>
-    <row r="35" spans="3:7">
-      <c r="C35" s="26" t="s">
-        <v>41</v>
-      </c>
-      <c r="D35" s="23" t="s">
+    <row r="35" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C35" s="25" t="s">
+        <v>38</v>
+      </c>
+      <c r="D35" s="20" t="s">
         <v>8</v>
       </c>
       <c r="E35" s="3" t="s">
-        <v>70</v>
+        <v>59</v>
       </c>
       <c r="F35" s="10"/>
       <c r="G35" s="4"/>
     </row>
-    <row r="36" spans="3:7">
-      <c r="C36" s="27"/>
-      <c r="D36" s="25"/>
+    <row r="36" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C36" s="26"/>
+      <c r="D36" s="21"/>
       <c r="E36" s="12" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="F36" s="10"/>
       <c r="G36" s="4"/>
     </row>
-    <row r="37" spans="3:7">
-      <c r="C37" s="23" t="s">
-        <v>38</v>
-      </c>
-      <c r="D37" s="23" t="s">
+    <row r="37" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C37" s="20" t="s">
+        <v>35</v>
+      </c>
+      <c r="D37" s="20" t="s">
         <v>19</v>
       </c>
       <c r="E37" s="3" t="s">
-        <v>66</v>
+        <v>57</v>
       </c>
       <c r="F37" s="10"/>
       <c r="G37" s="4"/>
     </row>
-    <row r="38" spans="3:7">
-      <c r="C38" s="25"/>
-      <c r="D38" s="25"/>
+    <row r="38" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C38" s="21"/>
+      <c r="D38" s="21"/>
       <c r="E38" s="3" t="s">
-        <v>75</v>
+        <v>64</v>
       </c>
       <c r="F38" s="10"/>
       <c r="G38" s="4"/>
     </row>
-    <row r="39" spans="3:7">
-      <c r="C39" s="23" t="s">
-        <v>46</v>
-      </c>
-      <c r="D39" s="23" t="s">
+    <row r="39" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C39" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="D39" s="20" t="s">
         <v>12</v>
       </c>
       <c r="E39" s="13" t="s">
-        <v>62</v>
+        <v>74</v>
       </c>
       <c r="F39" s="10" t="s">
-        <v>64</v>
+        <v>56</v>
       </c>
       <c r="G39" s="4"/>
     </row>
-    <row r="40" spans="3:7" ht="47.25">
-      <c r="C40" s="25"/>
-      <c r="D40" s="25"/>
+    <row r="40" spans="3:7" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="C40" s="21"/>
+      <c r="D40" s="21"/>
       <c r="E40" s="18" t="s">
-        <v>63</v>
+        <v>55</v>
       </c>
       <c r="F40" s="17" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="G40" s="4"/>
     </row>
-    <row r="41" spans="3:7">
-      <c r="C41" s="23" t="s">
-        <v>48</v>
-      </c>
-      <c r="D41" s="23" t="s">
+    <row r="41" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C41" s="20" t="s">
+        <v>45</v>
+      </c>
+      <c r="D41" s="20" t="s">
         <v>9</v>
       </c>
       <c r="E41" s="13" t="s">
-        <v>59</v>
-      </c>
-      <c r="F41" s="10" t="s">
-        <v>60</v>
+        <v>53</v>
+      </c>
+      <c r="F41" s="29" t="s">
+        <v>72</v>
       </c>
       <c r="G41" s="4"/>
     </row>
-    <row r="42" spans="3:7">
+    <row r="42" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C42" s="24"/>
       <c r="D42" s="24"/>
       <c r="E42" s="12" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
       <c r="F42" s="10"/>
       <c r="G42" s="4"/>
     </row>
-    <row r="43" spans="3:7">
+    <row r="43" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C43" s="24"/>
       <c r="D43" s="24"/>
       <c r="E43" s="12" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="F43" s="10"/>
       <c r="G43" s="4"/>
     </row>
-    <row r="44" spans="3:7">
-      <c r="C44" s="25"/>
-      <c r="D44" s="25"/>
+    <row r="44" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C44" s="21"/>
+      <c r="D44" s="21"/>
       <c r="E44" s="12" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="F44" s="10"/>
       <c r="G44" s="4"/>
     </row>
-    <row r="45" spans="3:7">
-      <c r="C45" s="23" t="s">
-        <v>44</v>
-      </c>
-      <c r="D45" s="23" t="s">
+    <row r="45" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C45" s="20" t="s">
+        <v>41</v>
+      </c>
+      <c r="D45" s="20" t="s">
         <v>10</v>
       </c>
       <c r="E45" s="13" t="s">
-        <v>25</v>
-      </c>
-      <c r="F45" s="10" t="s">
-        <v>65</v>
+        <v>22</v>
+      </c>
+      <c r="F45" s="29" t="s">
+        <v>73</v>
       </c>
       <c r="G45" s="4"/>
     </row>
-    <row r="46" spans="3:7">
-      <c r="C46" s="25"/>
-      <c r="D46" s="25"/>
+    <row r="46" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C46" s="21"/>
+      <c r="D46" s="21"/>
       <c r="E46" s="3"/>
       <c r="F46" s="10"/>
       <c r="G46" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="28">
-    <mergeCell ref="C45:C46"/>
-    <mergeCell ref="D24:D25"/>
-    <mergeCell ref="D26:D27"/>
-    <mergeCell ref="D28:D29"/>
-    <mergeCell ref="D39:D40"/>
-    <mergeCell ref="D45:D46"/>
+    <mergeCell ref="D17:D18"/>
+    <mergeCell ref="C19:C20"/>
+    <mergeCell ref="C28:C29"/>
+    <mergeCell ref="C30:C32"/>
+    <mergeCell ref="C33:C34"/>
+    <mergeCell ref="D22:D23"/>
     <mergeCell ref="D15:D16"/>
     <mergeCell ref="D41:D44"/>
     <mergeCell ref="D37:D38"/>
@@ -1487,12 +1490,12 @@
     <mergeCell ref="C26:C27"/>
     <mergeCell ref="C24:C25"/>
     <mergeCell ref="C22:C23"/>
-    <mergeCell ref="D17:D18"/>
-    <mergeCell ref="C19:C20"/>
-    <mergeCell ref="C28:C29"/>
-    <mergeCell ref="C30:C32"/>
-    <mergeCell ref="C33:C34"/>
-    <mergeCell ref="D22:D23"/>
+    <mergeCell ref="C45:C46"/>
+    <mergeCell ref="D24:D25"/>
+    <mergeCell ref="D26:D27"/>
+    <mergeCell ref="D28:D29"/>
+    <mergeCell ref="D39:D40"/>
+    <mergeCell ref="D45:D46"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <extLst>

</xml_diff>

<commit_message>
Race/Class powers chart miniupdate
</commit_message>
<xml_diff>
--- a/Sunken Temple/Ideas/Sunken Temple.xlsx
+++ b/Sunken Temple/Ideas/Sunken Temple.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="78">
   <si>
     <t>Dwarf</t>
   </si>
@@ -108,9 +108,6 @@
     <t>Resistant to all Magic attacks</t>
   </si>
   <si>
-    <t>Summon</t>
-  </si>
-  <si>
     <t>Flying</t>
   </si>
   <si>
@@ -247,6 +244,15 @@
   </si>
   <si>
     <t>Agility</t>
+  </si>
+  <si>
+    <t>bones</t>
+  </si>
+  <si>
+    <t>Uses (a certain number of) bones (per monster level) to sacrifice a monster, leaving no corpse (and no treasure) behind.  Player still gains experience.</t>
+  </si>
+  <si>
+    <t>Raise Dead</t>
   </si>
 </sst>
 </file>
@@ -468,7 +474,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -525,35 +531,38 @@
     <xf numFmtId="0" fontId="3" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="53">
@@ -945,8 +954,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C3:J46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B25" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+    <sheetView tabSelected="1" topLeftCell="B16" workbookViewId="0">
+      <selection activeCell="E33" sqref="E33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1087,7 +1096,7 @@
     </row>
     <row r="14" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C14" s="15" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D14" s="9" t="s">
         <v>18</v>
@@ -1103,54 +1112,54 @@
       </c>
     </row>
     <row r="15" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C15" s="22" t="s">
-        <v>40</v>
-      </c>
-      <c r="D15" s="22" t="s">
+      <c r="C15" s="21" t="s">
+        <v>39</v>
+      </c>
+      <c r="D15" s="21" t="s">
         <v>0</v>
       </c>
       <c r="E15" s="13" t="s">
-        <v>48</v>
-      </c>
-      <c r="F15" s="29" t="s">
-        <v>69</v>
+        <v>47</v>
+      </c>
+      <c r="F15" s="20" t="s">
+        <v>68</v>
       </c>
       <c r="G15" s="4"/>
     </row>
     <row r="16" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C16" s="23"/>
-      <c r="D16" s="23"/>
+      <c r="C16" s="22"/>
+      <c r="D16" s="22"/>
       <c r="E16" s="3"/>
       <c r="F16" s="10"/>
       <c r="G16" s="4"/>
     </row>
     <row r="17" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C17" s="22" t="s">
-        <v>39</v>
-      </c>
-      <c r="D17" s="22" t="s">
+      <c r="C17" s="21" t="s">
+        <v>38</v>
+      </c>
+      <c r="D17" s="21" t="s">
         <v>1</v>
       </c>
       <c r="E17" s="13" t="s">
-        <v>75</v>
-      </c>
-      <c r="F17" s="29" t="s">
-        <v>70</v>
+        <v>74</v>
+      </c>
+      <c r="F17" s="20" t="s">
+        <v>69</v>
       </c>
       <c r="G17" s="4"/>
     </row>
     <row r="18" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C18" s="23"/>
-      <c r="D18" s="23"/>
+      <c r="C18" s="22"/>
+      <c r="D18" s="22"/>
       <c r="E18" s="3"/>
       <c r="F18" s="10"/>
       <c r="G18" s="4"/>
     </row>
     <row r="19" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C19" s="22" t="s">
-        <v>42</v>
-      </c>
-      <c r="D19" s="22" t="s">
+      <c r="C19" s="21" t="s">
+        <v>41</v>
+      </c>
+      <c r="D19" s="21" t="s">
         <v>15</v>
       </c>
       <c r="E19" s="13" t="s">
@@ -1162,13 +1171,13 @@
       <c r="G19" s="4"/>
     </row>
     <row r="20" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C20" s="27"/>
-      <c r="D20" s="27"/>
+      <c r="C20" s="23"/>
+      <c r="D20" s="23"/>
       <c r="E20" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="F20" s="10" t="s">
         <v>46</v>
-      </c>
-      <c r="F20" s="10" t="s">
-        <v>47</v>
       </c>
       <c r="G20" s="4"/>
     </row>
@@ -1179,15 +1188,15 @@
         <v>23</v>
       </c>
       <c r="F21" s="10" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="G21" s="4"/>
     </row>
     <row r="22" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C22" s="28" t="s">
-        <v>32</v>
-      </c>
-      <c r="D22" s="22" t="s">
+      <c r="C22" s="29" t="s">
+        <v>31</v>
+      </c>
+      <c r="D22" s="21" t="s">
         <v>2</v>
       </c>
       <c r="E22" s="13" t="s">
@@ -1199,91 +1208,91 @@
       <c r="G22" s="4"/>
     </row>
     <row r="23" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C23" s="28"/>
-      <c r="D23" s="23"/>
+      <c r="C23" s="29"/>
+      <c r="D23" s="22"/>
       <c r="E23" s="3"/>
       <c r="F23" s="10"/>
       <c r="G23" s="4"/>
     </row>
     <row r="24" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C24" s="28" t="s">
-        <v>44</v>
-      </c>
-      <c r="D24" s="22" t="s">
+      <c r="C24" s="29" t="s">
+        <v>43</v>
+      </c>
+      <c r="D24" s="21" t="s">
         <v>3</v>
       </c>
       <c r="E24" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="F24" s="29" t="s">
-        <v>65</v>
+      <c r="F24" s="20" t="s">
+        <v>64</v>
       </c>
       <c r="G24" s="4"/>
     </row>
     <row r="25" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C25" s="28"/>
-      <c r="D25" s="23"/>
+      <c r="C25" s="29"/>
+      <c r="D25" s="22"/>
       <c r="E25" s="3"/>
       <c r="F25" s="10"/>
       <c r="G25" s="4"/>
     </row>
     <row r="26" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C26" s="28" t="s">
-        <v>31</v>
-      </c>
-      <c r="D26" s="22" t="s">
+      <c r="C26" s="29" t="s">
+        <v>30</v>
+      </c>
+      <c r="D26" s="21" t="s">
         <v>4</v>
       </c>
       <c r="E26" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="F26" s="29" t="s">
+      <c r="F26" s="20" t="s">
+        <v>65</v>
+      </c>
+      <c r="G26" s="4"/>
+    </row>
+    <row r="27" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C27" s="29"/>
+      <c r="D27" s="22"/>
+      <c r="E27" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="F27" s="20" t="s">
         <v>66</v>
       </c>
-      <c r="G26" s="4"/>
-    </row>
-    <row r="27" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C27" s="28"/>
-      <c r="D27" s="23"/>
-      <c r="E27" s="12" t="s">
-        <v>30</v>
-      </c>
-      <c r="F27" s="29" t="s">
-        <v>67</v>
-      </c>
       <c r="G27" s="4"/>
     </row>
     <row r="28" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C28" s="22" t="s">
-        <v>36</v>
-      </c>
-      <c r="D28" s="22" t="s">
+      <c r="C28" s="21" t="s">
+        <v>35</v>
+      </c>
+      <c r="D28" s="21" t="s">
         <v>5</v>
       </c>
       <c r="E28" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="F28" s="29" t="s">
-        <v>68</v>
+      <c r="F28" s="20" t="s">
+        <v>67</v>
       </c>
       <c r="G28" s="4"/>
     </row>
     <row r="29" spans="3:7" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="C29" s="23"/>
-      <c r="D29" s="23"/>
+      <c r="C29" s="22"/>
+      <c r="D29" s="22"/>
       <c r="E29" s="18" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F29" s="17" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="G29" s="4"/>
     </row>
     <row r="30" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C30" s="20" t="s">
-        <v>34</v>
-      </c>
-      <c r="D30" s="20" t="s">
+      <c r="C30" s="24" t="s">
+        <v>33</v>
+      </c>
+      <c r="D30" s="24" t="s">
         <v>6</v>
       </c>
       <c r="E30" s="3"/>
@@ -1291,189 +1300,195 @@
       <c r="G30" s="4"/>
     </row>
     <row r="31" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C31" s="24"/>
-      <c r="D31" s="24"/>
+      <c r="C31" s="25"/>
+      <c r="D31" s="25"/>
       <c r="E31" s="12" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F31" s="10"/>
       <c r="G31" s="4"/>
     </row>
     <row r="32" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C32" s="21"/>
-      <c r="D32" s="21"/>
+      <c r="C32" s="26"/>
+      <c r="D32" s="26"/>
       <c r="E32" s="12" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F32" s="10"/>
       <c r="G32" s="4"/>
     </row>
-    <row r="33" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C33" s="20" t="s">
-        <v>37</v>
-      </c>
-      <c r="D33" s="20" t="s">
+    <row r="33" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C33" s="24" t="s">
+        <v>36</v>
+      </c>
+      <c r="D33" s="24" t="s">
         <v>11</v>
       </c>
       <c r="E33" s="13" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="F33" s="10"/>
       <c r="G33" s="4"/>
-    </row>
-    <row r="34" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C34" s="21"/>
-      <c r="D34" s="21"/>
+      <c r="I33" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="34" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C34" s="26"/>
+      <c r="D34" s="26"/>
       <c r="E34" s="19" t="s">
-        <v>29</v>
+        <v>77</v>
       </c>
       <c r="F34" s="10" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G34" s="4"/>
     </row>
-    <row r="35" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C35" s="25" t="s">
-        <v>38</v>
-      </c>
-      <c r="D35" s="20" t="s">
+    <row r="35" spans="3:9" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="C35" s="27" t="s">
+        <v>37</v>
+      </c>
+      <c r="D35" s="24" t="s">
         <v>8</v>
       </c>
-      <c r="E35" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="F35" s="10"/>
+      <c r="E35" s="30" t="s">
+        <v>58</v>
+      </c>
+      <c r="F35" s="17" t="s">
+        <v>76</v>
+      </c>
       <c r="G35" s="4"/>
-    </row>
-    <row r="36" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C36" s="26"/>
-      <c r="D36" s="21"/>
-      <c r="E36" s="12" t="s">
-        <v>29</v>
-      </c>
+      <c r="I35" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="36" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C36" s="28"/>
+      <c r="D36" s="26"/>
+      <c r="E36" s="12"/>
       <c r="F36" s="10"/>
       <c r="G36" s="4"/>
     </row>
-    <row r="37" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C37" s="20" t="s">
-        <v>35</v>
-      </c>
-      <c r="D37" s="20" t="s">
+    <row r="37" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C37" s="24" t="s">
+        <v>34</v>
+      </c>
+      <c r="D37" s="24" t="s">
         <v>19</v>
       </c>
       <c r="E37" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F37" s="10"/>
       <c r="G37" s="4"/>
     </row>
-    <row r="38" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C38" s="21"/>
-      <c r="D38" s="21"/>
+    <row r="38" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C38" s="26"/>
+      <c r="D38" s="26"/>
       <c r="E38" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="F38" s="10"/>
       <c r="G38" s="4"/>
     </row>
-    <row r="39" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C39" s="20" t="s">
-        <v>43</v>
-      </c>
-      <c r="D39" s="20" t="s">
+    <row r="39" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C39" s="24" t="s">
+        <v>42</v>
+      </c>
+      <c r="D39" s="24" t="s">
         <v>12</v>
       </c>
       <c r="E39" s="13" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F39" s="10" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G39" s="4"/>
     </row>
-    <row r="40" spans="3:7" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="C40" s="21"/>
-      <c r="D40" s="21"/>
+    <row r="40" spans="3:9" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="C40" s="26"/>
+      <c r="D40" s="26"/>
       <c r="E40" s="18" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F40" s="17" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="G40" s="4"/>
     </row>
-    <row r="41" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C41" s="20" t="s">
-        <v>45</v>
-      </c>
-      <c r="D41" s="20" t="s">
+    <row r="41" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C41" s="24" t="s">
+        <v>44</v>
+      </c>
+      <c r="D41" s="24" t="s">
         <v>9</v>
       </c>
       <c r="E41" s="13" t="s">
+        <v>52</v>
+      </c>
+      <c r="F41" s="20" t="s">
+        <v>71</v>
+      </c>
+      <c r="G41" s="4"/>
+    </row>
+    <row r="42" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C42" s="25"/>
+      <c r="D42" s="25"/>
+      <c r="E42" s="12" t="s">
         <v>53</v>
-      </c>
-      <c r="F41" s="29" t="s">
-        <v>72</v>
-      </c>
-      <c r="G41" s="4"/>
-    </row>
-    <row r="42" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C42" s="24"/>
-      <c r="D42" s="24"/>
-      <c r="E42" s="12" t="s">
-        <v>54</v>
       </c>
       <c r="F42" s="10"/>
       <c r="G42" s="4"/>
     </row>
-    <row r="43" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C43" s="24"/>
-      <c r="D43" s="24"/>
+    <row r="43" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C43" s="25"/>
+      <c r="D43" s="25"/>
       <c r="E43" s="12" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F43" s="10"/>
       <c r="G43" s="4"/>
     </row>
-    <row r="44" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C44" s="21"/>
-      <c r="D44" s="21"/>
+    <row r="44" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C44" s="26"/>
+      <c r="D44" s="26"/>
       <c r="E44" s="12" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F44" s="10"/>
       <c r="G44" s="4"/>
     </row>
-    <row r="45" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C45" s="20" t="s">
-        <v>41</v>
-      </c>
-      <c r="D45" s="20" t="s">
+    <row r="45" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C45" s="24" t="s">
+        <v>40</v>
+      </c>
+      <c r="D45" s="24" t="s">
         <v>10</v>
       </c>
       <c r="E45" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="F45" s="29" t="s">
-        <v>73</v>
+      <c r="F45" s="20" t="s">
+        <v>72</v>
       </c>
       <c r="G45" s="4"/>
     </row>
-    <row r="46" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C46" s="21"/>
-      <c r="D46" s="21"/>
+    <row r="46" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C46" s="26"/>
+      <c r="D46" s="26"/>
       <c r="E46" s="3"/>
       <c r="F46" s="10"/>
       <c r="G46" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="28">
-    <mergeCell ref="D17:D18"/>
-    <mergeCell ref="C19:C20"/>
-    <mergeCell ref="C28:C29"/>
-    <mergeCell ref="C30:C32"/>
-    <mergeCell ref="C33:C34"/>
-    <mergeCell ref="D22:D23"/>
+    <mergeCell ref="C45:C46"/>
+    <mergeCell ref="D24:D25"/>
+    <mergeCell ref="D26:D27"/>
+    <mergeCell ref="D28:D29"/>
+    <mergeCell ref="D39:D40"/>
+    <mergeCell ref="D45:D46"/>
     <mergeCell ref="D15:D16"/>
     <mergeCell ref="D41:D44"/>
     <mergeCell ref="D37:D38"/>
@@ -1490,12 +1505,12 @@
     <mergeCell ref="C26:C27"/>
     <mergeCell ref="C24:C25"/>
     <mergeCell ref="C22:C23"/>
-    <mergeCell ref="C45:C46"/>
-    <mergeCell ref="D24:D25"/>
-    <mergeCell ref="D26:D27"/>
-    <mergeCell ref="D28:D29"/>
-    <mergeCell ref="D39:D40"/>
-    <mergeCell ref="D45:D46"/>
+    <mergeCell ref="D17:D18"/>
+    <mergeCell ref="C19:C20"/>
+    <mergeCell ref="C28:C29"/>
+    <mergeCell ref="C30:C32"/>
+    <mergeCell ref="C33:C34"/>
+    <mergeCell ref="D22:D23"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <extLst>

</xml_diff>